<commit_message>
Fix: Issue with drools not working
</commit_message>
<xml_diff>
--- a/src/main/java/com/samagra/orchestrator/Drools/OrchestratorRules.xlsx
+++ b/src/main/java/com/samagra/orchestrator/Drools/OrchestratorRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/chaks/experiments/java/comms/orchestrator/src/main/java/com/samagra/orchestrator/Drools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DEC6F-C377-ED4C-8A23-6797235F3982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB36671-B646-6741-8973-CFC28FABF0A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductOffering" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
   <si>
     <t>RuleSet</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>FAILED_TO_DELIVER</t>
+  </si>
+  <si>
+    <t>REPLIED</t>
+  </si>
+  <si>
+    <t>Add Form Transformer</t>
+  </si>
+  <si>
+    <t>"Form"</t>
+  </si>
+  <si>
+    <t>$xMessage.setChannelURI($param);</t>
+  </si>
+  <si>
+    <t>$xMessage.getChannelURI()</t>
   </si>
 </sst>
 </file>
@@ -433,15 +448,11 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -457,6 +468,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -785,17 +800,16 @@
     <col min="3" max="3" width="27.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
     <col min="5" max="5" width="29.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" style="1" customWidth="1"/>
-    <col min="11" max="17" width="11.5" style="1" customWidth="1"/>
-    <col min="18" max="28" width="10" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="14.5" style="1"/>
+    <col min="10" max="16" width="11.5" style="1" customWidth="1"/>
+    <col min="17" max="27" width="10" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -807,19 +821,19 @@
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
     </row>
-    <row r="2" spans="1:11" ht="37.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="37.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="34"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
     </row>
-    <row r="3" spans="1:11" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -831,20 +845,20 @@
       <c r="H3" s="27"/>
       <c r="I3" s="28"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="I4" s="28"/>
     </row>
-    <row r="5" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -853,22 +867,22 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="K5" s="9"/>
+      <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="39" t="s">
+    <row r="6" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="K6" s="9"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="13.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="13.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
         <v>2</v>
       </c>
@@ -893,22 +907,22 @@
       <c r="I7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:11" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="38"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
-      <c r="K8" s="9"/>
+      <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="17" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="17" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
       <c r="C9" s="14" t="s">
         <v>40</v>
@@ -920,19 +934,19 @@
         <v>35</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>37</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
@@ -961,7 +975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="18" t="s">
         <v>13</v>
       </c>
@@ -987,7 +1001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
         <v>15</v>
       </c>
@@ -1013,7 +1027,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>20</v>
       </c>
@@ -1035,17 +1049,23 @@
       <c r="H13" s="20"/>
       <c r="I13" s="21"/>
     </row>
-    <row r="14" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="22"/>
-      <c r="C14" s="4"/>
+    <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -1055,7 +1075,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="22"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1121,21 +1141,21 @@
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
       <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:13" ht="37.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="34"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:13" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -1153,14 +1173,14 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -1175,7 +1195,7 @@
       <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" ht="14" x14ac:dyDescent="0.2">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="40" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="31"/>
@@ -1184,7 +1204,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
+      <c r="I6" s="39"/>
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" ht="13.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1216,15 +1236,15 @@
     </row>
     <row r="8" spans="1:13" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="36"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" ht="17" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">

</xml_diff>